<commit_message>
Fix closing null value
</commit_message>
<xml_diff>
--- a/test/snap/readme.snap.xlsx
+++ b/test/snap/readme.snap.xlsx
@@ -25,9 +25,7 @@
       <c r="B2">
         <v>0.99</v>
       </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
+      <c r="C2"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>

<commit_message>
Add support for bold text
</commit_message>
<xml_diff>
--- a/test/snap/readme.snap.xlsx
+++ b/test/snap/readme.snap.xlsx
@@ -5,7 +5,7 @@
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -51,11 +51,11 @@
           <t>Sum</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>SUM(B1:B3)</f>
       </c>
-      <c r="C4">
-        <v>8</v>
+      <c r="C4" s="1">
+        <v>43102.642245</v>
       </c>
     </row>
   </sheetData>
@@ -65,13 +65,21 @@
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <!-- Date format -->
-    <numFmt numFmtId="165" formatCode="dd.mm.yyyy hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
     <!-- DateTime format -->
   </numFmts>
-  <fonts count="1">
-    <font/>
+  <fonts count="2">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -84,9 +92,10 @@
   <borders count="1">
     <border/>
   </borders>
-  <cellXfs count="2">
-    <xf numFmtId="0"/>
+  <cellXfs count="3">
+    <xf fontId="0" applyFont="1"/>
     <xf numFmtId="164" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1"/>
   </cellXfs>
 </styleSheet>
 </file>

</xml_diff>

<commit_message>
Add support for col options
</commit_message>
<xml_diff>
--- a/test/snap/readme.snap.xlsx
+++ b/test/snap/readme.snap.xlsx
@@ -3,8 +3,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D5"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" with="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -47,7 +47,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sum</t>
+          <t>Sum of all fruits</t>
         </is>
       </c>
       <c r="B4" s="2">
@@ -65,138 +65,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:AB1"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>J</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>O</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Q</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>U</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="X5" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>Z</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AA5" t="inlineStr">
         <is>
           <t>AA</t>
         </is>

</xml_diff>